<commit_message>
Adding Spreadsheet Writing Functionality
The program will no write the important data findings to the Sample Data
spreadsheet
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Sample Location</t>
   </si>
@@ -40,12 +40,16 @@
   </si>
   <si>
     <t>SampleText.txt</t>
+  </si>
+  <si>
+    <t>Full Text Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,45 +395,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>793.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.06305170239596469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginning of Sample Processing
First 4 files were chosen from the internet and processed for their
Collegiate Word Ratio (CWR). TODO: find a better method for sample
selection
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Sample Location</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -42,7 +39,55 @@
     <t>SampleText.txt</t>
   </si>
   <si>
-    <t>Full Text Location</t>
+    <t>Architercture-Messina.pdf</t>
+  </si>
+  <si>
+    <t>Full Text File Name</t>
+  </si>
+  <si>
+    <t>Sample File Name</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Messina, Culler, Pfeiffer…</t>
+  </si>
+  <si>
+    <t>The AGI Containment Problem-Yampolskiy.pdf</t>
+  </si>
+  <si>
+    <t>SampleText2.txt</t>
+  </si>
+  <si>
+    <t>The AGI Containment Problem</t>
+  </si>
+  <si>
+    <t>Babcock, Kramar, Yampolskiy</t>
+  </si>
+  <si>
+    <t>To The BestFriend-Collier.txt</t>
+  </si>
+  <si>
+    <t>SampleText3.txt</t>
+  </si>
+  <si>
+    <t>To The "Bestfriend" I decided I couldn't be friends with anymore</t>
+  </si>
+  <si>
+    <t>Alexandra Collier</t>
+  </si>
+  <si>
+    <t>SampleText4.txt</t>
+  </si>
+  <si>
+    <t>Generic anatomy of Escherichia coli 0157h7 outbreaks-Eppinger.pdf</t>
+  </si>
+  <si>
+    <t>Generic anatomy of Escherichia coli 0157h7 outbreaks</t>
+  </si>
+  <si>
+    <t>Eppinger,Mammel,Leclerc,Ravel,Cebula</t>
   </si>
 </sst>
 </file>
@@ -395,19 +440,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="43.26953125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="30.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.54296875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.26953125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="20.453125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="20.54296875" collapsed="true"/>
   </cols>
@@ -417,36 +462,114 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="n">
-        <v>793.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.06305170239596469</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>401</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>4.738154613466334E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>839</v>
+      </c>
+      <c r="F3">
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>4.6483909415971393E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>841</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>9.512485136741973E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="n">
+        <v>649.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.04314329738058552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>